<commit_message>
updates in factorial text
</commit_message>
<xml_diff>
--- a/data/factorial.xlsx
+++ b/data/factorial.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hkaur\Documents\GitHub\mixed-models-in-R\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A866A063-D463-46CC-8730-5D4B25E3BAC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB2B75B-6840-469F-8705-9742C2988413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{E4146260-9F13-4F91-B450-8F4900A41AF8}"/>
+    <workbookView xWindow="20370" yWindow="730" windowWidth="17350" windowHeight="12970" xr2:uid="{E4146260-9F13-4F91-B450-8F4900A41AF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$45</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,12 +39,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="8">
   <si>
     <t>animal</t>
-  </si>
-  <si>
-    <t>side</t>
   </si>
   <si>
     <t>location</t>
@@ -53,28 +50,19 @@
     <t>trt</t>
   </si>
   <si>
-    <t>retailday</t>
-  </si>
-  <si>
-    <t>b1</t>
-  </si>
-  <si>
-    <t>left</t>
-  </si>
-  <si>
     <t>superficial</t>
   </si>
   <si>
     <t>alt</t>
   </si>
   <si>
-    <t>right</t>
-  </si>
-  <si>
     <t>traditional</t>
   </si>
   <si>
     <t>deep</t>
+  </si>
+  <si>
+    <t>b_star</t>
   </si>
 </sst>
 </file>
@@ -431,220 +419,160 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68963A8F-CB85-49E9-AE21-AACCA411D780}">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.81640625" customWidth="1"/>
-    <col min="4" max="5" width="10.453125" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0</v>
-      </c>
-      <c r="F2">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2">
         <v>21.5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-      <c r="F3">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3">
         <v>20.100000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
+      <c r="B4" t="s">
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="D4">
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
+      <c r="B5" t="s">
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
-      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="D5">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>6</v>
+      <c r="B6" t="s">
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0</v>
-      </c>
-      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="D6">
         <v>16.8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0</v>
-      </c>
-      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="D7">
         <v>15.2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0</v>
-      </c>
-      <c r="F8">
+        <v>4</v>
+      </c>
+      <c r="D8">
         <v>18.2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0</v>
-      </c>
-      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="D9">
         <v>18.5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0</v>
-      </c>
-      <c r="F10">
+        <v>4</v>
+      </c>
+      <c r="D10">
         <v>20.3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>3</v>
       </c>
@@ -652,79 +580,55 @@
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0</v>
-      </c>
-      <c r="F11">
+        <v>4</v>
+      </c>
+      <c r="D11">
         <v>24.5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="1">
-        <v>0</v>
-      </c>
-      <c r="F12">
+        <v>5</v>
+      </c>
+      <c r="D12">
         <v>22.3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="1">
-        <v>0</v>
-      </c>
-      <c r="F13">
+        <v>5</v>
+      </c>
+      <c r="D13">
         <v>19.7</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>4</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="1">
-        <v>0</v>
-      </c>
-      <c r="F14">
+        <v>5</v>
+      </c>
+      <c r="D14">
         <v>17.3</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>4</v>
       </c>
@@ -732,79 +636,55 @@
         <v>6</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="1">
-        <v>0</v>
-      </c>
-      <c r="F15">
+        <v>5</v>
+      </c>
+      <c r="D15">
         <v>18.5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>4</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="1">
-        <v>0</v>
-      </c>
-      <c r="F16">
+        <v>4</v>
+      </c>
+      <c r="D16">
         <v>17.5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>4</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="1">
-        <v>0</v>
-      </c>
-      <c r="F17">
+        <v>4</v>
+      </c>
+      <c r="D17">
         <v>22.6</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>5</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="1">
-        <v>0</v>
-      </c>
-      <c r="F18">
+        <v>4</v>
+      </c>
+      <c r="D18">
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>5</v>
       </c>
@@ -812,59 +692,41 @@
         <v>6</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="1">
-        <v>0</v>
-      </c>
-      <c r="F19">
+        <v>4</v>
+      </c>
+      <c r="D19">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>5</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="1">
-        <v>0</v>
-      </c>
-      <c r="F20">
+        <v>5</v>
+      </c>
+      <c r="D20">
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>5</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="1">
-        <v>0</v>
-      </c>
-      <c r="F21">
+        <v>5</v>
+      </c>
+      <c r="D21">
         <v>17.8</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>6</v>
       </c>
@@ -872,99 +734,69 @@
         <v>6</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" s="1">
-        <v>0</v>
-      </c>
-      <c r="F22">
+        <v>5</v>
+      </c>
+      <c r="D22">
         <v>17.100000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>6</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" s="1">
-        <v>0</v>
-      </c>
-      <c r="F23">
+        <v>5</v>
+      </c>
+      <c r="D23">
         <v>14.2</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>6</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24" s="1">
-        <v>0</v>
-      </c>
-      <c r="F24">
+        <v>4</v>
+      </c>
+      <c r="D24">
         <v>17.8</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>6</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" s="1">
-        <v>0</v>
-      </c>
-      <c r="F25">
+        <v>4</v>
+      </c>
+      <c r="D25">
         <v>19.2</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>7</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" s="1">
-        <v>0</v>
-      </c>
-      <c r="F26">
+        <v>4</v>
+      </c>
+      <c r="D26">
         <v>13.2</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>7</v>
       </c>
@@ -972,79 +804,55 @@
         <v>6</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" s="1">
-        <v>0</v>
-      </c>
-      <c r="F27">
+        <v>4</v>
+      </c>
+      <c r="D27">
         <v>19.8</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>7</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E28" s="1">
-        <v>0</v>
-      </c>
-      <c r="F28">
+        <v>5</v>
+      </c>
+      <c r="D28">
         <v>16.5</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>7</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29" s="1">
-        <v>0</v>
-      </c>
-      <c r="F29">
+        <v>5</v>
+      </c>
+      <c r="D29">
         <v>18.7</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>8</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E30" s="1">
-        <v>0</v>
-      </c>
-      <c r="F30">
+        <v>5</v>
+      </c>
+      <c r="D30">
         <v>13.7</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>8</v>
       </c>
@@ -1052,79 +860,55 @@
         <v>6</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E31" s="1">
-        <v>0</v>
-      </c>
-      <c r="F31">
+        <v>5</v>
+      </c>
+      <c r="D31">
         <v>18.3</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>8</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E32" s="1">
-        <v>0</v>
-      </c>
-      <c r="F32">
+        <v>4</v>
+      </c>
+      <c r="D32">
         <v>15.5</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>8</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E33" s="1">
-        <v>0</v>
-      </c>
-      <c r="F33">
+        <v>4</v>
+      </c>
+      <c r="D33">
         <v>19.399999999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>9</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E34" s="1">
-        <v>0</v>
-      </c>
-      <c r="F34">
+        <v>4</v>
+      </c>
+      <c r="D34">
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>9</v>
       </c>
@@ -1132,79 +916,55 @@
         <v>6</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E35" s="1">
-        <v>0</v>
-      </c>
-      <c r="F35">
+        <v>4</v>
+      </c>
+      <c r="D35">
         <v>11.2</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>9</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E36" s="1">
-        <v>0</v>
-      </c>
-      <c r="F36">
+        <v>5</v>
+      </c>
+      <c r="D36">
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>9</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E37" s="1">
-        <v>0</v>
-      </c>
-      <c r="F37">
+        <v>5</v>
+      </c>
+      <c r="D37">
         <v>15.4</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>10</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E38" s="1">
-        <v>0</v>
-      </c>
-      <c r="F38">
+        <v>5</v>
+      </c>
+      <c r="D38">
         <v>19.8</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>10</v>
       </c>
@@ -1212,79 +972,55 @@
         <v>6</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E39" s="1">
-        <v>0</v>
-      </c>
-      <c r="F39">
+        <v>5</v>
+      </c>
+      <c r="D39">
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>10</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E40" s="1">
-        <v>0</v>
-      </c>
-      <c r="F40">
+        <v>4</v>
+      </c>
+      <c r="D40">
         <v>15.3</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>10</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E41" s="1">
-        <v>0</v>
-      </c>
-      <c r="F41">
+        <v>4</v>
+      </c>
+      <c r="D41">
         <v>16.600000000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>11</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E42" s="1">
-        <v>0</v>
-      </c>
-      <c r="F42">
+        <v>4</v>
+      </c>
+      <c r="D42">
         <v>14.5</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>11</v>
       </c>
@@ -1292,64 +1028,42 @@
         <v>6</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E43" s="1">
-        <v>0</v>
-      </c>
-      <c r="F43">
+        <v>4</v>
+      </c>
+      <c r="D43">
         <v>19.399999999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>11</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E44" s="1">
-        <v>0</v>
-      </c>
-      <c r="F44">
+        <v>5</v>
+      </c>
+      <c r="D44">
         <v>15.7</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>11</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E45" s="1">
-        <v>0</v>
-      </c>
-      <c r="F45">
+        <v>5</v>
+      </c>
+      <c r="D45">
         <v>18.600000000000001</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F45" xr:uid="{68963A8F-CB85-49E9-AE21-AACCA411D780}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F45">
-      <sortCondition ref="E1:E45"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:D45" xr:uid="{68963A8F-CB85-49E9-AE21-AACCA411D780}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>